<commit_message>
The first complete working version.
</commit_message>
<xml_diff>
--- a/doc/VAT_CAP4_hid_protocol.xlsx
+++ b/doc/VAT_CAP4_hid_protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Freia\freia-drop\08 Equipment\Cryostat02_Gersemi\09 Controls and Software\VAT_Reheater_Valves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24EF14B1-9F59-4D4A-9350-5949AD841834}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{05A6221E-8004-4846-A464-DDEE345A7644}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18580" windowHeight="7440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="57">
   <si>
     <t>Function</t>
   </si>
@@ -183,12 +183,21 @@
   <si>
     <t>F5</t>
   </si>
+  <si>
+    <t>Get end switch state</t>
+  </si>
+  <si>
+    <t>Par ID: 10100000</t>
+  </si>
+  <si>
+    <t>0C</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,8 +234,13 @@
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Monospace"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +263,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0F0E9"/>
+        <bgColor rgb="FFF0F0E9"/>
       </patternFill>
     </fill>
   </fills>
@@ -351,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -362,6 +382,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -588,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -613,74 +634,74 @@
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:66" ht="14.25" customHeight="1">
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="13" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="14"/>
-      <c r="AG2" s="14"/>
-      <c r="AH2" s="14"/>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="14"/>
-      <c r="AK2" s="14"/>
-      <c r="AL2" s="14"/>
-      <c r="AM2" s="14"/>
-      <c r="AN2" s="14"/>
-      <c r="AO2" s="14"/>
-      <c r="AP2" s="14"/>
-      <c r="AQ2" s="14"/>
-      <c r="AR2" s="14"/>
-      <c r="AS2" s="14"/>
-      <c r="AT2" s="14"/>
-      <c r="AU2" s="14"/>
-      <c r="AV2" s="14"/>
-      <c r="AW2" s="14"/>
-      <c r="AX2" s="14"/>
-      <c r="AY2" s="14"/>
-      <c r="AZ2" s="14"/>
-      <c r="BA2" s="14"/>
-      <c r="BB2" s="14"/>
-      <c r="BC2" s="14"/>
-      <c r="BD2" s="14"/>
-      <c r="BE2" s="14"/>
-      <c r="BF2" s="14"/>
-      <c r="BG2" s="14"/>
-      <c r="BH2" s="14"/>
-      <c r="BI2" s="14"/>
-      <c r="BJ2" s="14"/>
-      <c r="BK2" s="14"/>
-      <c r="BL2" s="14"/>
-      <c r="BM2" s="14"/>
-      <c r="BN2" s="14"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="15"/>
+      <c r="AI2" s="15"/>
+      <c r="AJ2" s="15"/>
+      <c r="AK2" s="15"/>
+      <c r="AL2" s="15"/>
+      <c r="AM2" s="15"/>
+      <c r="AN2" s="15"/>
+      <c r="AO2" s="15"/>
+      <c r="AP2" s="15"/>
+      <c r="AQ2" s="15"/>
+      <c r="AR2" s="15"/>
+      <c r="AS2" s="15"/>
+      <c r="AT2" s="15"/>
+      <c r="AU2" s="15"/>
+      <c r="AV2" s="15"/>
+      <c r="AW2" s="15"/>
+      <c r="AX2" s="15"/>
+      <c r="AY2" s="15"/>
+      <c r="AZ2" s="15"/>
+      <c r="BA2" s="15"/>
+      <c r="BB2" s="15"/>
+      <c r="BC2" s="15"/>
+      <c r="BD2" s="15"/>
+      <c r="BE2" s="15"/>
+      <c r="BF2" s="15"/>
+      <c r="BG2" s="15"/>
+      <c r="BH2" s="15"/>
+      <c r="BI2" s="15"/>
+      <c r="BJ2" s="15"/>
+      <c r="BK2" s="15"/>
+      <c r="BL2" s="15"/>
+      <c r="BM2" s="15"/>
+      <c r="BN2" s="15"/>
     </row>
     <row r="3" spans="1:66" ht="14.25" customHeight="1">
       <c r="B3" s="1" t="s">
@@ -6035,6 +6056,12 @@
       <c r="J58" s="2"/>
     </row>
     <row r="59" spans="1:66" ht="14.25" customHeight="1">
+      <c r="A59" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -6045,44 +6072,472 @@
       <c r="J59" s="2"/>
     </row>
     <row r="60" spans="1:66" ht="14.25" customHeight="1">
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
+      <c r="A60" s="3"/>
+      <c r="B60" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" s="10">
+        <v>18</v>
+      </c>
+      <c r="F60" s="10">
+        <v>0</v>
+      </c>
+      <c r="G60" s="10">
+        <v>15</v>
+      </c>
+      <c r="H60" s="10">
+        <v>0</v>
+      </c>
+      <c r="I60" s="10">
+        <v>0</v>
+      </c>
+      <c r="J60" s="10">
+        <v>0</v>
+      </c>
+      <c r="K60" s="10">
+        <v>70</v>
+      </c>
+      <c r="L60" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M60" s="10">
+        <v>30</v>
+      </c>
+      <c r="N60" s="10">
+        <v>42</v>
+      </c>
+      <c r="O60" s="10">
+        <v>31</v>
+      </c>
+      <c r="P60" s="10">
+        <v>30</v>
+      </c>
+      <c r="Q60" s="10">
+        <v>31</v>
+      </c>
+      <c r="R60" s="10">
+        <v>30</v>
+      </c>
+      <c r="S60" s="10">
+        <v>30</v>
+      </c>
+      <c r="T60" s="10">
+        <v>30</v>
+      </c>
+      <c r="U60" s="10">
+        <v>30</v>
+      </c>
+      <c r="V60" s="10">
+        <v>30</v>
+      </c>
+      <c r="W60" s="10">
+        <v>30</v>
+      </c>
+      <c r="X60" s="10">
+        <v>30</v>
+      </c>
+      <c r="Y60" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z60" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA60" s="3"/>
+      <c r="AB60" s="3"/>
+      <c r="AC60" s="3"/>
+      <c r="AD60" s="3"/>
+      <c r="AE60" s="3"/>
+      <c r="AF60" s="3"/>
+      <c r="AG60" s="3"/>
+      <c r="AH60" s="3"/>
+      <c r="AI60" s="3"/>
+      <c r="AJ60" s="3"/>
+      <c r="AK60" s="3"/>
+      <c r="AL60" s="3"/>
+      <c r="AM60" s="3"/>
+      <c r="AN60" s="3"/>
+      <c r="AO60" s="3"/>
+      <c r="AP60" s="3"/>
+      <c r="AQ60" s="3"/>
     </row>
     <row r="61" spans="1:66" ht="14.25" customHeight="1">
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
+      <c r="A61" s="3"/>
+      <c r="B61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="5" t="str">
+        <f t="shared" ref="C61:Z61" si="18">IF(HEX2DEC(C60)&gt;0, CHAR(HEX2DEC(C60))," ")</f>
+        <v>_x000C_</v>
+      </c>
+      <c r="D61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>_x001A_</v>
+      </c>
+      <c r="E61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>_x0018_</v>
+      </c>
+      <c r="F61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>_x0015_</v>
+      </c>
+      <c r="H61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>p</v>
+      </c>
+      <c r="L61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>:</v>
+      </c>
+      <c r="M61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="N61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>B</v>
+      </c>
+      <c r="O61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="P61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="R61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="T61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="U61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="V61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="W61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="X61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Y61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>_x000D_</v>
+      </c>
+      <c r="Z61" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">
+</v>
+      </c>
+      <c r="AA61" s="5"/>
+      <c r="AB61" s="5"/>
+      <c r="AC61" s="3"/>
+      <c r="AD61" s="3"/>
+      <c r="AE61" s="3"/>
+      <c r="AF61" s="3"/>
+      <c r="AG61" s="3"/>
+      <c r="AH61" s="3"/>
+      <c r="AI61" s="3"/>
+      <c r="AJ61" s="3"/>
+      <c r="AK61" s="3"/>
+      <c r="AL61" s="3"/>
+      <c r="AM61" s="3"/>
+      <c r="AN61" s="3"/>
+      <c r="AO61" s="3"/>
+      <c r="AP61" s="3"/>
+      <c r="AQ61" s="3"/>
     </row>
     <row r="62" spans="1:66" ht="14.25" customHeight="1">
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
+      <c r="A62" s="6"/>
+      <c r="B62" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F62" s="10">
+        <v>0</v>
+      </c>
+      <c r="G62" s="10">
+        <v>15</v>
+      </c>
+      <c r="H62" s="10">
+        <v>0</v>
+      </c>
+      <c r="I62" s="10">
+        <v>0</v>
+      </c>
+      <c r="J62" s="10">
+        <v>0</v>
+      </c>
+      <c r="K62" s="10">
+        <v>70</v>
+      </c>
+      <c r="L62" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M62" s="10">
+        <v>30</v>
+      </c>
+      <c r="N62" s="10">
+        <v>30</v>
+      </c>
+      <c r="O62" s="10">
+        <v>30</v>
+      </c>
+      <c r="P62" s="10">
+        <v>42</v>
+      </c>
+      <c r="Q62" s="10">
+        <v>31</v>
+      </c>
+      <c r="R62" s="10">
+        <v>30</v>
+      </c>
+      <c r="S62" s="10">
+        <v>31</v>
+      </c>
+      <c r="T62" s="10">
+        <v>30</v>
+      </c>
+      <c r="U62" s="10">
+        <v>30</v>
+      </c>
+      <c r="V62" s="10">
+        <v>30</v>
+      </c>
+      <c r="W62" s="10">
+        <v>30</v>
+      </c>
+      <c r="X62" s="10">
+        <v>30</v>
+      </c>
+      <c r="Y62" s="10">
+        <v>30</v>
+      </c>
+      <c r="Z62" s="10">
+        <v>30</v>
+      </c>
+      <c r="AA62" s="10">
+        <v>30</v>
+      </c>
+      <c r="AB62" s="10">
+        <v>31</v>
+      </c>
+      <c r="AC62" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD62" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE62" s="7"/>
+      <c r="AF62" s="7"/>
+      <c r="AG62" s="7"/>
+      <c r="AH62" s="7"/>
+      <c r="AI62" s="7"/>
+      <c r="AJ62" s="7"/>
+      <c r="AK62" s="6"/>
+      <c r="AL62" s="6"/>
+      <c r="AM62" s="6"/>
+      <c r="AN62" s="6"/>
+      <c r="AO62" s="6"/>
+      <c r="AP62" s="6"/>
+      <c r="AQ62" s="6"/>
     </row>
     <row r="63" spans="1:66" ht="14.25" customHeight="1">
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
+      <c r="A63" s="6"/>
+      <c r="B63" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="6" t="str">
+        <f t="shared" ref="C63:AJ63" si="19">IF(HEX2DEC(C62)&gt;0, CHAR(HEX2DEC(C62))," ")</f>
+        <v>_x000C_</v>
+      </c>
+      <c r="D63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>_x001A_</v>
+      </c>
+      <c r="E63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>_x001C_</v>
+      </c>
+      <c r="F63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>_x0015_</v>
+      </c>
+      <c r="H63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>p</v>
+      </c>
+      <c r="L63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>:</v>
+      </c>
+      <c r="M63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="N63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>B</v>
+      </c>
+      <c r="Q63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="R63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="T63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="V63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="W63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="X63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Z63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AA63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AB63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AC63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v>_x000D_</v>
+      </c>
+      <c r="AD63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">
+</v>
+      </c>
+      <c r="AE63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ63" s="6" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK63" s="6"/>
+      <c r="AL63" s="6"/>
+      <c r="AM63" s="6"/>
+      <c r="AN63" s="6"/>
+      <c r="AO63" s="6"/>
+      <c r="AP63" s="6"/>
+      <c r="AQ63" s="6"/>
     </row>
     <row r="64" spans="1:66" ht="14.25" customHeight="1">
       <c r="C64" s="2"/>

</xml_diff>